<commit_message>
fixed createing from excel to accept const cells
</commit_message>
<xml_diff>
--- a/modelx/tests/core/data/testdata.xlsx
+++ b/modelx/tests/core/data/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27450" windowHeight="13040" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27450" windowHeight="13040"/>
   </bookViews>
   <sheets>
     <sheet name="TestTables" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="25">
   <si>
     <t>Param</t>
     <phoneticPr fontId="1"/>
@@ -74,12 +74,52 @@
     <t>Sex</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>Test data for SpaceContainer.create_space_from_excel</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Const Table</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Cells1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Cells2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Product</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Cells1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Cells2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Const Table</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +141,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -110,7 +157,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -159,13 +206,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -182,6 +251,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -488,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:Z62"/>
+  <dimension ref="C3:AD67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O59" sqref="O59:X62"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -504,12 +585,17 @@
     <col min="23" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:26" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="3" spans="3:30" ht="14.25" x14ac:dyDescent="0.15">
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="3:26" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="7" spans="3:30" x14ac:dyDescent="0.2">
+      <c r="AC7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="3:30" ht="14.25" x14ac:dyDescent="0.15">
       <c r="N8" s="2" t="s">
         <v>0</v>
       </c>
@@ -535,8 +621,14 @@
         <v>12</v>
       </c>
       <c r="Z8" s="5"/>
-    </row>
-    <row r="9" spans="3:26" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="AC8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD8" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="3:30" ht="14.25" x14ac:dyDescent="0.15">
       <c r="C9" s="2" t="s">
         <v>0</v>
       </c>
@@ -589,8 +681,14 @@
       <c r="Z9" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="3:26" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="AC9" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD9" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="3:30" ht="14.25" x14ac:dyDescent="0.15">
       <c r="C10" s="2">
         <v>0</v>
       </c>
@@ -659,7 +757,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="11" spans="3:26" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="11" spans="3:30" ht="14.25" x14ac:dyDescent="0.15">
       <c r="C11" s="2">
         <f>C10+1</f>
         <v>1</v>
@@ -732,7 +830,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="12" spans="3:26" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="12" spans="3:30" ht="14.25" x14ac:dyDescent="0.15">
       <c r="C12" s="2">
         <f t="shared" ref="C12:C25" si="13">C11+1</f>
         <v>2</v>
@@ -805,7 +903,7 @@
         <v>3002</v>
       </c>
     </row>
-    <row r="13" spans="3:26" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="13" spans="3:30" ht="14.25" x14ac:dyDescent="0.15">
       <c r="C13" s="2">
         <f t="shared" si="13"/>
         <v>3</v>
@@ -878,7 +976,7 @@
         <v>3003</v>
       </c>
     </row>
-    <row r="14" spans="3:26" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="14" spans="3:30" ht="14.25" x14ac:dyDescent="0.15">
       <c r="C14" s="2">
         <f t="shared" si="13"/>
         <v>4</v>
@@ -951,7 +1049,7 @@
         <v>3004</v>
       </c>
     </row>
-    <row r="15" spans="3:26" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="15" spans="3:30" ht="14.25" x14ac:dyDescent="0.15">
       <c r="C15" s="2">
         <f t="shared" si="13"/>
         <v>5</v>
@@ -1024,7 +1122,7 @@
         <v>3005</v>
       </c>
     </row>
-    <row r="16" spans="3:26" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="16" spans="3:30" ht="14.25" x14ac:dyDescent="0.15">
       <c r="C16" s="2">
         <f t="shared" si="13"/>
         <v>6</v>
@@ -2201,7 +2299,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="44" spans="3:19" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="44" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C44" s="2" t="s">
         <v>11</v>
       </c>
@@ -2270,7 +2368,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="45" spans="3:19" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="45" spans="3:19" x14ac:dyDescent="0.2">
       <c r="C45" s="2" t="s">
         <v>12</v>
       </c>
@@ -2339,7 +2437,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="49" spans="3:24" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="49" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C49" s="2" t="s">
         <v>0</v>
       </c>
@@ -2694,7 +2792,7 @@
         <v>3015</v>
       </c>
     </row>
-    <row r="57" spans="3:24" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="57" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C57" s="3" t="s">
         <v>9</v>
       </c>
@@ -2778,7 +2876,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="3:24" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="58" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C58" s="2" t="s">
         <v>7</v>
       </c>
@@ -3192,6 +3290,22 @@
       <c r="X62" s="2">
         <f t="shared" si="42"/>
         <v>4009</v>
+      </c>
+    </row>
+    <row r="66" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C66" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D66" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C67" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D67" s="2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3213,15 +3327,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:X37"/>
+  <dimension ref="C1:X43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="3:8" ht="14" x14ac:dyDescent="0.2">
+    <row r="1" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="3:13" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
@@ -3236,8 +3358,17 @@
         <v>12</v>
       </c>
       <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="3:8" ht="14" x14ac:dyDescent="0.2">
+      <c r="K3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="3:13" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C4" s="3"/>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -3254,8 +3385,17 @@
       <c r="H4" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="3:8" ht="14" x14ac:dyDescent="0.2">
+      <c r="K4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="6">
+        <v>1</v>
+      </c>
+      <c r="M4" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="3:13" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C5" s="3">
         <v>0</v>
       </c>
@@ -3278,8 +3418,19 @@
         <f>G5+1000</f>
         <v>3000</v>
       </c>
-    </row>
-    <row r="6" spans="3:8" ht="14" x14ac:dyDescent="0.2">
+      <c r="K5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="6">
+        <f>L4+1</f>
+        <v>2</v>
+      </c>
+      <c r="M5" s="6">
+        <f>M4+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" ht="14" x14ac:dyDescent="0.2">
       <c r="C6" s="3">
         <f>C5+1</f>
         <v>1</v>
@@ -3288,7 +3439,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" ref="E6:E24" si="0">1000+$C6</f>
+        <f t="shared" ref="E6:E14" si="0">1000+$C6</f>
         <v>1001</v>
       </c>
       <c r="F6" s="2">
@@ -3296,7 +3447,7 @@
         <v>2001</v>
       </c>
       <c r="G6" s="2">
-        <f t="shared" ref="G6:G24" si="2">2000+$C6</f>
+        <f t="shared" ref="G6:G14" si="2">2000+$C6</f>
         <v>2001</v>
       </c>
       <c r="H6" s="2">
@@ -3304,7 +3455,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="7" spans="3:8" ht="14" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:13" ht="14" x14ac:dyDescent="0.2">
       <c r="C7" s="3">
         <f t="shared" ref="C7:C24" si="4">C6+1</f>
         <v>2</v>
@@ -3329,7 +3480,7 @@
         <v>3002</v>
       </c>
     </row>
-    <row r="8" spans="3:8" ht="14" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:13" ht="14" x14ac:dyDescent="0.2">
       <c r="C8" s="3">
         <f t="shared" si="4"/>
         <v>3</v>
@@ -3354,7 +3505,7 @@
         <v>3003</v>
       </c>
     </row>
-    <row r="9" spans="3:8" ht="14" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:13" ht="14" x14ac:dyDescent="0.2">
       <c r="C9" s="3">
         <f t="shared" si="4"/>
         <v>4</v>
@@ -3379,7 +3530,7 @@
         <v>3004</v>
       </c>
     </row>
-    <row r="10" spans="3:8" ht="14" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:13" ht="14" x14ac:dyDescent="0.2">
       <c r="C10" s="3">
         <f t="shared" si="4"/>
         <v>5</v>
@@ -3404,7 +3555,7 @@
         <v>3005</v>
       </c>
     </row>
-    <row r="11" spans="3:8" ht="14" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:13" ht="14" x14ac:dyDescent="0.2">
       <c r="C11" s="3">
         <f t="shared" si="4"/>
         <v>6</v>
@@ -3429,7 +3580,7 @@
         <v>3006</v>
       </c>
     </row>
-    <row r="12" spans="3:8" ht="14" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:13" ht="14" x14ac:dyDescent="0.2">
       <c r="C12" s="3">
         <f t="shared" si="4"/>
         <v>7</v>
@@ -3454,7 +3605,7 @@
         <v>3007</v>
       </c>
     </row>
-    <row r="13" spans="3:8" ht="14" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:13" ht="14" x14ac:dyDescent="0.2">
       <c r="C13" s="3">
         <f t="shared" si="4"/>
         <v>8</v>
@@ -3479,7 +3630,7 @@
         <v>3008</v>
       </c>
     </row>
-    <row r="14" spans="3:8" ht="14" x14ac:dyDescent="0.2">
+    <row r="14" spans="3:13" ht="14" x14ac:dyDescent="0.2">
       <c r="C14" s="3">
         <f t="shared" si="4"/>
         <v>9</v>
@@ -3504,7 +3655,7 @@
         <v>3009</v>
       </c>
     </row>
-    <row r="15" spans="3:8" ht="14" x14ac:dyDescent="0.2">
+    <row r="15" spans="3:13" ht="14" x14ac:dyDescent="0.2">
       <c r="C15" s="3">
         <v>0</v>
       </c>
@@ -3528,7 +3679,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="16" spans="3:8" ht="14" x14ac:dyDescent="0.2">
+    <row r="16" spans="3:13" ht="14" x14ac:dyDescent="0.2">
       <c r="C16" s="3">
         <f t="shared" si="4"/>
         <v>1</v>
@@ -3906,7 +4057,7 @@
       </c>
     </row>
     <row r="34" spans="3:24" ht="14" x14ac:dyDescent="0.2">
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="8" t="s">
         <v>11</v>
       </c>
       <c r="D34" s="2" t="s">
@@ -3994,7 +4145,7 @@
       </c>
     </row>
     <row r="35" spans="3:24" ht="14" x14ac:dyDescent="0.2">
-      <c r="C35" s="5"/>
+      <c r="C35" s="9"/>
       <c r="D35" s="2" t="s">
         <v>4</v>
       </c>
@@ -4080,7 +4231,7 @@
       </c>
     </row>
     <row r="36" spans="3:24" ht="14" x14ac:dyDescent="0.2">
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="8" t="s">
         <v>12</v>
       </c>
       <c r="D36" s="2" t="s">
@@ -4103,7 +4254,7 @@
         <v>2003</v>
       </c>
       <c r="I36" s="2">
-        <f t="shared" ref="I36:X36" si="13">2000+I$32</f>
+        <f t="shared" ref="I36:N36" si="13">2000+I$32</f>
         <v>2004</v>
       </c>
       <c r="J36" s="2">
@@ -4168,7 +4319,7 @@
       </c>
     </row>
     <row r="37" spans="3:24" ht="14" x14ac:dyDescent="0.2">
-      <c r="C37" s="5"/>
+      <c r="C37" s="9"/>
       <c r="D37" s="2" t="s">
         <v>4</v>
       </c>
@@ -4251,6 +4402,41 @@
       <c r="X37" s="2">
         <f t="shared" si="15"/>
         <v>4009</v>
+      </c>
+    </row>
+    <row r="41" spans="3:24" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C41" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="3:24" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C42" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" s="6">
+        <v>1</v>
+      </c>
+      <c r="E42" s="6">
+        <f>D42+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="3:24" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="C43" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D43" s="6">
+        <v>2</v>
+      </c>
+      <c r="E43" s="6">
+        <f>D43+1</f>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test wit empty prams for createing from excel
</commit_message>
<xml_diff>
--- a/modelx/tests/core/data/testdata.xlsx
+++ b/modelx/tests/core/data/testdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="30">
   <si>
     <t>Param</t>
     <phoneticPr fontId="1"/>
@@ -112,6 +112,26 @@
   </si>
   <si>
     <t>Const Table</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Null Parameters</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Product</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Year</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Cells1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Cells2</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -247,17 +267,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -569,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:AD67"/>
+  <dimension ref="C3:AJ74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L71" sqref="L71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -585,50 +605,65 @@
     <col min="23" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:30" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="3" spans="3:36" ht="14.25" x14ac:dyDescent="0.15">
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="3:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:36" x14ac:dyDescent="0.2">
       <c r="AC7" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="3:30" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="AG7" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="3:36" ht="14.25" x14ac:dyDescent="0.15">
       <c r="N8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="O8" s="4" t="s">
+      <c r="O8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="4" t="s">
+      <c r="P8" s="7"/>
+      <c r="Q8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="R8" s="5"/>
+      <c r="R8" s="7"/>
       <c r="U8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="V8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="W8" s="4" t="s">
+      <c r="W8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="X8" s="5"/>
-      <c r="Y8" s="4" t="s">
+      <c r="X8" s="7"/>
+      <c r="Y8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="Z8" s="5"/>
+      <c r="Z8" s="7"/>
       <c r="AC8" s="2" t="s">
         <v>17</v>
       </c>
       <c r="AD8" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="3:30" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="AG8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AH8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AI8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ8" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="3:36" ht="14.25" x14ac:dyDescent="0.15">
       <c r="C9" s="2" t="s">
         <v>0</v>
       </c>
@@ -687,8 +722,17 @@
       <c r="AD9" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="3:30" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="AG9" s="2"/>
+      <c r="AH9" s="2"/>
+      <c r="AI9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="2">
+        <f>AI9+1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="3:36" ht="14.25" x14ac:dyDescent="0.15">
       <c r="C10" s="2">
         <v>0</v>
       </c>
@@ -756,8 +800,20 @@
         <f>Y10+1000</f>
         <v>3000</v>
       </c>
-    </row>
-    <row r="11" spans="3:30" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="AG10" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH10" s="2"/>
+      <c r="AI10" s="2">
+        <f>AI9+1</f>
+        <v>1</v>
+      </c>
+      <c r="AJ10" s="2">
+        <f>AI10+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="3:36" ht="14.25" x14ac:dyDescent="0.15">
       <c r="C11" s="2">
         <f>C10+1</f>
         <v>1</v>
@@ -829,8 +885,20 @@
         <f t="shared" ref="Z11:Z29" si="12">Y11+1000</f>
         <v>3001</v>
       </c>
-    </row>
-    <row r="12" spans="3:30" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="AG11" s="2"/>
+      <c r="AH11" s="2">
+        <v>2</v>
+      </c>
+      <c r="AI11" s="2">
+        <f>AI10+1</f>
+        <v>2</v>
+      </c>
+      <c r="AJ11" s="2">
+        <f>AJ10+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="3:36" ht="14.25" x14ac:dyDescent="0.15">
       <c r="C12" s="2">
         <f t="shared" ref="C12:C25" si="13">C11+1</f>
         <v>2</v>
@@ -903,7 +971,7 @@
         <v>3002</v>
       </c>
     </row>
-    <row r="13" spans="3:30" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="13" spans="3:36" ht="14.25" x14ac:dyDescent="0.15">
       <c r="C13" s="2">
         <f t="shared" si="13"/>
         <v>3</v>
@@ -976,7 +1044,7 @@
         <v>3003</v>
       </c>
     </row>
-    <row r="14" spans="3:30" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="14" spans="3:36" ht="14.25" x14ac:dyDescent="0.15">
       <c r="C14" s="2">
         <f t="shared" si="13"/>
         <v>4</v>
@@ -1049,7 +1117,7 @@
         <v>3004</v>
       </c>
     </row>
-    <row r="15" spans="3:30" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="15" spans="3:36" ht="14.25" x14ac:dyDescent="0.15">
       <c r="C15" s="2">
         <f t="shared" si="13"/>
         <v>5</v>
@@ -1122,7 +1190,7 @@
         <v>3005</v>
       </c>
     </row>
-    <row r="16" spans="3:30" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="16" spans="3:36" ht="14.25" x14ac:dyDescent="0.15">
       <c r="C16" s="2">
         <f t="shared" si="13"/>
         <v>6</v>
@@ -2509,7 +2577,7 @@
       </c>
     </row>
     <row r="50" spans="3:24" x14ac:dyDescent="0.2">
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D50" s="2" t="s">
@@ -2581,7 +2649,7 @@
       </c>
     </row>
     <row r="51" spans="3:24" x14ac:dyDescent="0.2">
-      <c r="C51" s="5"/>
+      <c r="C51" s="7"/>
       <c r="D51" s="2" t="s">
         <v>4</v>
       </c>
@@ -2651,7 +2719,7 @@
       </c>
     </row>
     <row r="52" spans="3:24" x14ac:dyDescent="0.2">
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D52" s="2" t="s">
@@ -2723,7 +2791,7 @@
       </c>
     </row>
     <row r="53" spans="3:24" x14ac:dyDescent="0.2">
-      <c r="C53" s="5"/>
+      <c r="C53" s="7"/>
       <c r="D53" s="2" t="s">
         <v>4</v>
       </c>
@@ -2945,7 +3013,7 @@
       </c>
     </row>
     <row r="59" spans="3:24" x14ac:dyDescent="0.2">
-      <c r="C59" s="4" t="s">
+      <c r="C59" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D59" s="2" t="s">
@@ -3033,7 +3101,7 @@
       </c>
     </row>
     <row r="60" spans="3:24" x14ac:dyDescent="0.2">
-      <c r="C60" s="5"/>
+      <c r="C60" s="7"/>
       <c r="D60" s="2" t="s">
         <v>4</v>
       </c>
@@ -3119,7 +3187,7 @@
       </c>
     </row>
     <row r="61" spans="3:24" x14ac:dyDescent="0.2">
-      <c r="C61" s="4" t="s">
+      <c r="C61" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D61" s="2" t="s">
@@ -3207,7 +3275,7 @@
       </c>
     </row>
     <row r="62" spans="3:24" x14ac:dyDescent="0.2">
-      <c r="C62" s="5"/>
+      <c r="C62" s="7"/>
       <c r="D62" s="2" t="s">
         <v>4</v>
       </c>
@@ -3292,7 +3360,7 @@
         <v>4009</v>
       </c>
     </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C66" s="2" t="s">
         <v>17</v>
       </c>
@@ -3300,12 +3368,65 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C67" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D67" s="2">
         <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C71" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2">
+        <v>1</v>
+      </c>
+      <c r="F71" s="2"/>
+    </row>
+    <row r="72" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C72" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C73" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D73" s="2">
+        <v>0</v>
+      </c>
+      <c r="E73" s="2">
+        <f>D73+1</f>
+        <v>1</v>
+      </c>
+      <c r="F73" s="2">
+        <f>E73+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C74" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D74" s="2">
+        <f>D73+1</f>
+        <v>1</v>
+      </c>
+      <c r="E74" s="2">
+        <f>E73+1</f>
+        <v>2</v>
+      </c>
+      <c r="F74" s="2">
+        <f>E74+1</f>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -3350,21 +3471,21 @@
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="4" t="s">
+      <c r="F3" s="7"/>
+      <c r="G3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="K3" s="6" t="s">
+      <c r="H3" s="7"/>
+      <c r="K3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3385,13 +3506,13 @@
       <c r="H4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="4">
         <v>1</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="4">
         <v>2</v>
       </c>
     </row>
@@ -3418,14 +3539,14 @@
         <f>G5+1000</f>
         <v>3000</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="4">
         <f>L4+1</f>
         <v>2</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="4">
         <f>M4+1</f>
         <v>3</v>
       </c>
@@ -4405,36 +4526,36 @@
       </c>
     </row>
     <row r="41" spans="3:24" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="E41" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="42" spans="3:24" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D42" s="4">
         <v>1</v>
       </c>
-      <c r="E42" s="6">
+      <c r="E42" s="4">
         <f>D42+1</f>
         <v>2</v>
       </c>
     </row>
     <row r="43" spans="3:24" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D43" s="4">
         <v>2</v>
       </c>
-      <c r="E43" s="6">
+      <c r="E43" s="4">
         <f>D43+1</f>
         <v>3</v>
       </c>

</xml_diff>